<commit_message>
[lakhan] resume upload added daily change only path
</commit_message>
<xml_diff>
--- a/TestData/NaukariLoginDetails.xlsx
+++ b/TestData/NaukariLoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakha\eclipse\Fresh-eclipse-workspace\Naukari\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32AF062-CFE8-4EC9-852D-B6CD0C8DEC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D647D706-1204-4AB7-834E-D48FA1756704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{D30C8ADD-A122-4CCD-9BF8-2CFC78D6DB52}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>8rPk_H.cZ_jmuEP</t>
   </si>
   <si>
     <t>lakhansadewar@gmail.com</t>
+  </si>
+  <si>
+    <t>Over three years of experience as a software quality analyst, worked on designing and maintaining scripts for automation testing. Knowledge of Maven, Jenkins, GIT, SQL &amp; UNIX. Skilled in Java, Selenium WebDriver and Data-Driven Framework.</t>
   </si>
 </sst>
 </file>
@@ -66,9 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404B9A6E-D704-4EDA-89DB-FF43D94D8145}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -395,12 +397,15 @@
     <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Lsa] Friday resume Update
</commit_message>
<xml_diff>
--- a/TestData/NaukariLoginDetails.xlsx
+++ b/TestData/NaukariLoginDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lakha\eclipse\Fresh-eclipse-workspace\Naukari\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D647D706-1204-4AB7-834E-D48FA1756704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DC2778-0871-4EFB-9D0F-1DC23BB71E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{D30C8ADD-A122-4CCD-9BF8-2CFC78D6DB52}"/>
+    <workbookView xWindow="30450" yWindow="1650" windowWidth="14400" windowHeight="10545" xr2:uid="{D30C8ADD-A122-4CCD-9BF8-2CFC78D6DB52}"/>
   </bookViews>
   <sheets>
     <sheet name="naukaridata" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <t>lakhansadewar@gmail.com</t>
   </si>
   <si>
-    <t>Over three years of experience as a software quality analyst, worked on designing and maintaining scripts for automation testing. Knowledge of Maven, Jenkins, GIT, SQL &amp; UNIX. Skilled in Java, Selenium WebDriver and Data-Driven Framework.</t>
+    <t>Software quality analyst with 3.2 years of experience in software quality processes, Involved in end-to-end features testing. Skills in Automation testing, Manual UI Testing, Database and API Testing.</t>
   </si>
 </sst>
 </file>
@@ -388,13 +388,14 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="172.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>